<commit_message>
Removed Drops from Query, Added trigger and SPROC, updated SD
</commit_message>
<xml_diff>
--- a/group2_DoomsdaySDFinal.xlsx
+++ b/group2_DoomsdaySDFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bette\Desktop\School\Data\Group Work\doomsday-prep-group-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F43390-4F47-49ED-AA0D-BED040B96E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7638D3-1EBA-4941-AF15-18B91A3AFB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECD664E1-0401-4CD1-9F2B-897F2ADAE0C9}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="16410" windowHeight="14145" xr2:uid="{ECD664E1-0401-4CD1-9F2B-897F2ADAE0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
   <si>
     <t>cameron_brandt</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>(Standard User)</t>
+  </si>
+  <si>
+    <t>usp_UpdateInventoryAtSurvivorShelter</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF07CD7F-E538-4410-8CEA-3FF2143D5092}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,152 +613,173 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>14</v>
       </c>
-      <c r="B33" t="s">
-        <v>6</v>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>